<commit_message>
Refactor codebase for simplicity and API consistency
Major changes:
- Consolidate user_settings loading in config.py with single helper function
- Unify data access API: get_safe_value -> _get_safe_value (internal),
  extend COLUMN_ALIASES for PI/TS columns
- Rewrite excel_generator.py to use xlwings for better image/format preservation
- Simplify template_engine.py by marking most functions as deprecated
- Keep history.py using openpyxl for reading (more stable than xlwings COM)
- Update all CLI files and generators to use get_value with internal keys
- Add create_pi.py CLI for Proforma Invoice generation
- Add logging_config.py module for centralized logging setup
- Update tests to work with new xlwings-based API

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/templates/transaction_statement.xlsx
+++ b/templates/transaction_statement.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rotork-my.sharepoint.com/personal/jeongtaek_bang_rotork_com/Documents/바탕 화면/업무/NOAH ACTUATION/purchaseOrderAutomation/templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rotork-my.sharepoint.com/personal/jeongtaek_bang_rotork_com/Documents/바탕 화면/업무/NOAH ACTUATION/noahAutomation/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="48" documentId="11_848294B80D5E6C82562DAD935A2AD0F07A586A18" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DAF7CE82-191F-4FF6-B14D-CD4C31820749}"/>
+  <xr:revisionPtr revIDLastSave="246" documentId="11_848294B80D5E6C82562DAD935A2AD0F07A586A18" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B05ECC6B-DEDD-5CCB-8F9B-B7C0F511010E}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -340,6 +340,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -374,9 +377,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -472,6 +472,10 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -781,31 +785,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
     </row>
     <row r="2" spans="1:8">
       <c r="B2" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E2" s="16" t="s">
+      <c r="E2" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="F2" s="16"/>
-      <c r="G2" s="17" t="s">
+      <c r="F2" s="17"/>
+      <c r="G2" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="18"/>
+      <c r="H2" s="19"/>
     </row>
     <row r="3" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="B3" s="27" t="s">
+      <c r="B3" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="20"/>
+      <c r="C3" s="21"/>
       <c r="E3" s="3" t="s">
         <v>3</v>
       </c>
@@ -820,22 +824,22 @@
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
+      <c r="B4" s="21"/>
+      <c r="C4" s="21"/>
       <c r="E4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="26" t="s">
+      <c r="F4" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="G4" s="26"/>
-      <c r="H4" s="26"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
     </row>
     <row r="5" spans="1:8">
-      <c r="B5" s="24" t="s">
+      <c r="B5" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="20"/>
+      <c r="C5" s="21"/>
       <c r="E5" s="3" t="s">
         <v>8</v>
       </c>
@@ -850,18 +854,18 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="17.25">
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="20"/>
+      <c r="C7" s="21"/>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="6"/>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="7"/>
-      <c r="B10" s="25"/>
-      <c r="C10" s="20"/>
+      <c r="B10" s="26"/>
+      <c r="C10" s="21"/>
       <c r="D10" s="2"/>
       <c r="E10" s="8"/>
     </row>
@@ -892,7 +896,7 @@
       </c>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="28">
+      <c r="A13" s="15">
         <v>46038</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -918,7 +922,7 @@
       </c>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="28">
+      <c r="A14" s="15">
         <v>46038</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -974,14 +978,14 @@
       <c r="C25" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="E25" s="23" t="s">
+      <c r="E25" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="F25" s="22"/>
-      <c r="G25" s="21">
+      <c r="F25" s="23"/>
+      <c r="G25" s="22">
         <v>12408000</v>
       </c>
-      <c r="H25" s="22"/>
+      <c r="H25" s="23"/>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="13" t="s">

</xml_diff>

<commit_message>
v2.4: Add FI/PL templates, merged TS, refactor & optimize
- Add Final Invoice generator (fi_generator.py, create_fi.py)
- Add Packing List template
- Add merged transaction statement for monthly billing (--merge)
- Dispatch date-based TS dates instead of today
- Refactor: xlwings batch operations (96-97% COM call reduction)
- Refactor: XlConstants, xlwings_app_context, utils dedup
- Fix: path traversal security in cli_common.py
- Fix: xlwings .formula 2D tuple handling
- Add tests: cli_common, config, excel_helpers (47+ tests)
- Add docs: OPERATION_GUIDE, POWER_QUERY
- Update .gitignore for generated_fi/, generated_pi/

Co-Authored-By: Claude Opus 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/templates/transaction_statement.xlsx
+++ b/templates/transaction_statement.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rotork-my.sharepoint.com/personal/jeongtaek_bang_rotork_com/Documents/바탕 화면/업무/NOAH ACTUATION/noahAutomation/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="246" documentId="11_848294B80D5E6C82562DAD935A2AD0F07A586A18" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B05ECC6B-DEDD-5CCB-8F9B-B7C0F511010E}"/>
+  <xr:revisionPtr revIDLastSave="257" documentId="11_848294B80D5E6C82562DAD935A2AD0F07A586A18" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1D0FCABB-C63A-4AF9-A9AB-9637B606E5C1}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="거래명세표" sheetId="1" r:id="rId1"/>
@@ -159,7 +159,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="2">
     <numFmt numFmtId="176" formatCode="\₩#,##0"/>
     <numFmt numFmtId="177" formatCode="m&quot;월&quot;\ d&quot;일&quot;"/>
@@ -314,7 +314,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -359,13 +359,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -378,12 +371,26 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="표준" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{89A86B0A-9F4D-4F82-86B2-6FF46202E18B}"/>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -472,10 +479,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -769,7 +772,7 @@
   <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="160" zoomScaleNormal="100" zoomScaleSheetLayoutView="160" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -806,7 +809,7 @@
       <c r="H2" s="19"/>
     </row>
     <row r="3" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="25" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="21"/>
@@ -829,14 +832,14 @@
       <c r="E4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="27" t="s">
+      <c r="F4" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
     </row>
     <row r="5" spans="1:8">
-      <c r="B5" s="25" t="s">
+      <c r="B5" s="22" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="21"/>
@@ -864,7 +867,7 @@
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="7"/>
-      <c r="B10" s="26"/>
+      <c r="B10" s="23"/>
       <c r="C10" s="21"/>
       <c r="D10" s="2"/>
       <c r="E10" s="8"/>
@@ -978,14 +981,14 @@
       <c r="C25" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="E25" s="24" t="s">
+      <c r="E25" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="F25" s="23"/>
-      <c r="G25" s="22">
+      <c r="F25" s="27"/>
+      <c r="G25" s="28">
         <v>12408000</v>
       </c>
-      <c r="H25" s="23"/>
+      <c r="H25" s="29"/>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="13" t="s">
@@ -997,12 +1000,12 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="G25:H25"/>
     <mergeCell ref="E1:H1"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="B7:C7"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="E25:F25"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="F4:H4"/>

</xml_diff>